<commit_message>
read and update operation condtion
</commit_message>
<xml_diff>
--- a/Data/npcc.xlsx
+++ b/Data/npcc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EERL\NY-Simple-Net\Baseline-powergrid-model-for-NY\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2B27A7-D115-453F-8094-E17235F36BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7358B8EF-3613-49EC-8B46-F24512F47C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5988" yWindow="3048" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29604" yWindow="1116" windowWidth="23040" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="645">
   <si>
     <t>idx</t>
   </si>
@@ -1965,6 +1965,9 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -5276,8 +5279,8 @@
   <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M142" sqref="M142"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O89" sqref="O89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5367,8 +5370,8 @@
       <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="M2" t="s">
+        <v>644</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -5411,8 +5414,8 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3">
-        <v>0</v>
+      <c r="M3" t="s">
+        <v>644</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -5455,8 +5458,8 @@
       <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>0</v>
+      <c r="M4" t="s">
+        <v>644</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -5499,8 +5502,8 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="M5" t="s">
+        <v>644</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -5543,8 +5546,8 @@
       <c r="L6">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>0</v>
+      <c r="M6" t="s">
+        <v>644</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -5587,8 +5590,8 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>0</v>
+      <c r="M7" t="s">
+        <v>644</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -5631,8 +5634,8 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>0</v>
+      <c r="M8" t="s">
+        <v>644</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -5675,8 +5678,8 @@
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9">
-        <v>0</v>
+      <c r="M9" t="s">
+        <v>644</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -5719,8 +5722,8 @@
       <c r="L10">
         <v>1</v>
       </c>
-      <c r="M10">
-        <v>0</v>
+      <c r="M10" t="s">
+        <v>644</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -5763,8 +5766,8 @@
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11">
-        <v>0</v>
+      <c r="M11" t="s">
+        <v>644</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -5807,8 +5810,8 @@
       <c r="L12">
         <v>1</v>
       </c>
-      <c r="M12">
-        <v>0</v>
+      <c r="M12" t="s">
+        <v>644</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -5851,8 +5854,8 @@
       <c r="L13">
         <v>1</v>
       </c>
-      <c r="M13">
-        <v>0</v>
+      <c r="M13" t="s">
+        <v>644</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -5895,8 +5898,8 @@
       <c r="L14">
         <v>1</v>
       </c>
-      <c r="M14">
-        <v>0</v>
+      <c r="M14" t="s">
+        <v>644</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -5939,8 +5942,8 @@
       <c r="L15">
         <v>1</v>
       </c>
-      <c r="M15">
-        <v>0</v>
+      <c r="M15" t="s">
+        <v>644</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -5983,8 +5986,8 @@
       <c r="L16">
         <v>1</v>
       </c>
-      <c r="M16">
-        <v>0</v>
+      <c r="M16" t="s">
+        <v>644</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -6027,8 +6030,8 @@
       <c r="L17">
         <v>1</v>
       </c>
-      <c r="M17">
-        <v>0</v>
+      <c r="M17" t="s">
+        <v>644</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -6071,8 +6074,8 @@
       <c r="L18">
         <v>1</v>
       </c>
-      <c r="M18">
-        <v>0</v>
+      <c r="M18" t="s">
+        <v>644</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -6115,8 +6118,8 @@
       <c r="L19">
         <v>1</v>
       </c>
-      <c r="M19">
-        <v>0</v>
+      <c r="M19" t="s">
+        <v>644</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -6159,8 +6162,8 @@
       <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20">
-        <v>0</v>
+      <c r="M20" t="s">
+        <v>644</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -6203,8 +6206,8 @@
       <c r="L21">
         <v>1</v>
       </c>
-      <c r="M21">
-        <v>0</v>
+      <c r="M21" t="s">
+        <v>644</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -6247,8 +6250,8 @@
       <c r="L22">
         <v>1</v>
       </c>
-      <c r="M22">
-        <v>0</v>
+      <c r="M22" t="s">
+        <v>644</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -6291,8 +6294,8 @@
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="M23">
-        <v>0</v>
+      <c r="M23" t="s">
+        <v>644</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -6335,8 +6338,8 @@
       <c r="L24">
         <v>1</v>
       </c>
-      <c r="M24">
-        <v>0</v>
+      <c r="M24" t="s">
+        <v>644</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -6379,8 +6382,8 @@
       <c r="L25">
         <v>1</v>
       </c>
-      <c r="M25">
-        <v>0</v>
+      <c r="M25" t="s">
+        <v>644</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -6423,8 +6426,8 @@
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="M26">
-        <v>0</v>
+      <c r="M26" t="s">
+        <v>644</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -6467,8 +6470,8 @@
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="M27">
-        <v>0</v>
+      <c r="M27" t="s">
+        <v>644</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -6511,8 +6514,8 @@
       <c r="L28">
         <v>1</v>
       </c>
-      <c r="M28">
-        <v>0</v>
+      <c r="M28" t="s">
+        <v>644</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -6555,8 +6558,8 @@
       <c r="L29">
         <v>1</v>
       </c>
-      <c r="M29">
-        <v>0</v>
+      <c r="M29" t="s">
+        <v>644</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -6599,8 +6602,8 @@
       <c r="L30">
         <v>1</v>
       </c>
-      <c r="M30">
-        <v>0</v>
+      <c r="M30" t="s">
+        <v>644</v>
       </c>
       <c r="N30">
         <v>1</v>
@@ -6643,8 +6646,8 @@
       <c r="L31">
         <v>1</v>
       </c>
-      <c r="M31">
-        <v>0</v>
+      <c r="M31" t="s">
+        <v>644</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -6687,8 +6690,8 @@
       <c r="L32">
         <v>1</v>
       </c>
-      <c r="M32">
-        <v>0</v>
+      <c r="M32" t="s">
+        <v>644</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -6731,8 +6734,8 @@
       <c r="L33">
         <v>1</v>
       </c>
-      <c r="M33">
-        <v>0</v>
+      <c r="M33" t="s">
+        <v>644</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -6775,8 +6778,8 @@
       <c r="L34">
         <v>1</v>
       </c>
-      <c r="M34">
-        <v>0</v>
+      <c r="M34" t="s">
+        <v>644</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -6819,8 +6822,8 @@
       <c r="L35">
         <v>1</v>
       </c>
-      <c r="M35">
-        <v>0</v>
+      <c r="M35" t="s">
+        <v>644</v>
       </c>
       <c r="N35">
         <v>1</v>
@@ -6863,8 +6866,8 @@
       <c r="L36">
         <v>1</v>
       </c>
-      <c r="M36">
-        <v>0</v>
+      <c r="M36" t="s">
+        <v>644</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -6907,8 +6910,8 @@
       <c r="L37">
         <v>1</v>
       </c>
-      <c r="M37">
-        <v>0</v>
+      <c r="M37" t="s">
+        <v>644</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -6951,8 +6954,8 @@
       <c r="L38">
         <v>4</v>
       </c>
-      <c r="M38">
-        <v>0</v>
+      <c r="M38" t="s">
+        <v>644</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -6995,8 +6998,8 @@
       <c r="L39">
         <v>4</v>
       </c>
-      <c r="M39">
-        <v>0</v>
+      <c r="M39" t="s">
+        <v>644</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -7039,8 +7042,8 @@
       <c r="L40">
         <v>4</v>
       </c>
-      <c r="M40">
-        <v>0</v>
+      <c r="M40" t="s">
+        <v>644</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -7083,8 +7086,8 @@
       <c r="L41">
         <v>4</v>
       </c>
-      <c r="M41">
-        <v>0</v>
+      <c r="M41" t="s">
+        <v>644</v>
       </c>
       <c r="N41">
         <v>1</v>
@@ -7127,8 +7130,8 @@
       <c r="L42">
         <v>4</v>
       </c>
-      <c r="M42">
-        <v>0</v>
+      <c r="M42" t="s">
+        <v>644</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -7171,8 +7174,8 @@
       <c r="L43">
         <v>4</v>
       </c>
-      <c r="M43">
-        <v>0</v>
+      <c r="M43" t="s">
+        <v>644</v>
       </c>
       <c r="N43">
         <v>1</v>
@@ -7215,8 +7218,8 @@
       <c r="L44">
         <v>4</v>
       </c>
-      <c r="M44">
-        <v>0</v>
+      <c r="M44" t="s">
+        <v>644</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -7259,8 +7262,8 @@
       <c r="L45">
         <v>4</v>
       </c>
-      <c r="M45">
-        <v>0</v>
+      <c r="M45" t="s">
+        <v>644</v>
       </c>
       <c r="N45">
         <v>1</v>
@@ -7303,8 +7306,8 @@
       <c r="L46">
         <v>4</v>
       </c>
-      <c r="M46">
-        <v>0</v>
+      <c r="M46" t="s">
+        <v>644</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -7347,8 +7350,8 @@
       <c r="L47">
         <v>4</v>
       </c>
-      <c r="M47">
-        <v>0</v>
+      <c r="M47" t="s">
+        <v>644</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -7391,8 +7394,8 @@
       <c r="L48">
         <v>4</v>
       </c>
-      <c r="M48">
-        <v>0</v>
+      <c r="M48" t="s">
+        <v>644</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -7435,8 +7438,8 @@
       <c r="L49">
         <v>4</v>
       </c>
-      <c r="M49">
-        <v>0</v>
+      <c r="M49" t="s">
+        <v>644</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -7479,8 +7482,8 @@
       <c r="L50">
         <v>4</v>
       </c>
-      <c r="M50">
-        <v>0</v>
+      <c r="M50" t="s">
+        <v>644</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -7523,8 +7526,8 @@
       <c r="L51">
         <v>4</v>
       </c>
-      <c r="M51">
-        <v>0</v>
+      <c r="M51" t="s">
+        <v>644</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -7567,8 +7570,8 @@
       <c r="L52">
         <v>4</v>
       </c>
-      <c r="M52">
-        <v>0</v>
+      <c r="M52" t="s">
+        <v>644</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -7611,8 +7614,8 @@
       <c r="L53">
         <v>4</v>
       </c>
-      <c r="M53">
-        <v>0</v>
+      <c r="M53" t="s">
+        <v>644</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -7655,8 +7658,8 @@
       <c r="L54">
         <v>4</v>
       </c>
-      <c r="M54">
-        <v>0</v>
+      <c r="M54" t="s">
+        <v>644</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -7699,8 +7702,8 @@
       <c r="L55">
         <v>4</v>
       </c>
-      <c r="M55">
-        <v>0</v>
+      <c r="M55" t="s">
+        <v>644</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -7743,8 +7746,8 @@
       <c r="L56">
         <v>4</v>
       </c>
-      <c r="M56">
-        <v>0</v>
+      <c r="M56" t="s">
+        <v>644</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -7787,8 +7790,8 @@
       <c r="L57">
         <v>4</v>
       </c>
-      <c r="M57">
-        <v>0</v>
+      <c r="M57" t="s">
+        <v>644</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -7831,8 +7834,8 @@
       <c r="L58">
         <v>4</v>
       </c>
-      <c r="M58">
-        <v>0</v>
+      <c r="M58" t="s">
+        <v>644</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -7875,8 +7878,8 @@
       <c r="L59">
         <v>4</v>
       </c>
-      <c r="M59">
-        <v>0</v>
+      <c r="M59" t="s">
+        <v>644</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -7919,8 +7922,8 @@
       <c r="L60">
         <v>4</v>
       </c>
-      <c r="M60">
-        <v>0</v>
+      <c r="M60" t="s">
+        <v>644</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -7963,8 +7966,8 @@
       <c r="L61">
         <v>4</v>
       </c>
-      <c r="M61">
-        <v>0</v>
+      <c r="M61" t="s">
+        <v>644</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -8007,8 +8010,8 @@
       <c r="L62">
         <v>4</v>
       </c>
-      <c r="M62">
-        <v>0</v>
+      <c r="M62" t="s">
+        <v>644</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -8051,8 +8054,8 @@
       <c r="L63">
         <v>4</v>
       </c>
-      <c r="M63">
-        <v>0</v>
+      <c r="M63" t="s">
+        <v>644</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -8095,8 +8098,8 @@
       <c r="L64">
         <v>4</v>
       </c>
-      <c r="M64">
-        <v>0</v>
+      <c r="M64" t="s">
+        <v>644</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -8139,8 +8142,8 @@
       <c r="L65">
         <v>4</v>
       </c>
-      <c r="M65">
-        <v>0</v>
+      <c r="M65" t="s">
+        <v>644</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -8183,8 +8186,8 @@
       <c r="L66">
         <v>4</v>
       </c>
-      <c r="M66">
-        <v>0</v>
+      <c r="M66" t="s">
+        <v>644</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -8227,8 +8230,8 @@
       <c r="L67">
         <v>4</v>
       </c>
-      <c r="M67">
-        <v>0</v>
+      <c r="M67" t="s">
+        <v>644</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -8271,8 +8274,8 @@
       <c r="L68">
         <v>4</v>
       </c>
-      <c r="M68">
-        <v>0</v>
+      <c r="M68" t="s">
+        <v>644</v>
       </c>
       <c r="N68">
         <v>1</v>
@@ -8315,8 +8318,8 @@
       <c r="L69">
         <v>5</v>
       </c>
-      <c r="M69">
-        <v>0</v>
+      <c r="M69" t="s">
+        <v>644</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -8359,8 +8362,8 @@
       <c r="L70">
         <v>5</v>
       </c>
-      <c r="M70">
-        <v>0</v>
+      <c r="M70" t="s">
+        <v>644</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -8403,8 +8406,8 @@
       <c r="L71">
         <v>5</v>
       </c>
-      <c r="M71">
-        <v>0</v>
+      <c r="M71" t="s">
+        <v>644</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -8447,8 +8450,8 @@
       <c r="L72">
         <v>5</v>
       </c>
-      <c r="M72">
-        <v>0</v>
+      <c r="M72" t="s">
+        <v>644</v>
       </c>
       <c r="N72">
         <v>1</v>
@@ -8491,8 +8494,8 @@
       <c r="L73">
         <v>5</v>
       </c>
-      <c r="M73">
-        <v>0</v>
+      <c r="M73" t="s">
+        <v>644</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -8535,8 +8538,8 @@
       <c r="L74">
         <v>5</v>
       </c>
-      <c r="M74">
-        <v>0</v>
+      <c r="M74" t="s">
+        <v>644</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -8579,8 +8582,8 @@
       <c r="L75">
         <v>5</v>
       </c>
-      <c r="M75">
-        <v>0</v>
+      <c r="M75" t="s">
+        <v>644</v>
       </c>
       <c r="N75">
         <v>1</v>
@@ -8623,8 +8626,8 @@
       <c r="L76">
         <v>5</v>
       </c>
-      <c r="M76">
-        <v>0</v>
+      <c r="M76" t="s">
+        <v>644</v>
       </c>
       <c r="N76">
         <v>1</v>
@@ -8667,8 +8670,8 @@
       <c r="L77">
         <v>5</v>
       </c>
-      <c r="M77">
-        <v>0</v>
+      <c r="M77" t="s">
+        <v>644</v>
       </c>
       <c r="N77">
         <v>1</v>
@@ -8711,8 +8714,8 @@
       <c r="L78">
         <v>5</v>
       </c>
-      <c r="M78">
-        <v>0</v>
+      <c r="M78" t="s">
+        <v>644</v>
       </c>
       <c r="N78">
         <v>1</v>
@@ -8755,8 +8758,8 @@
       <c r="L79">
         <v>6</v>
       </c>
-      <c r="M79">
-        <v>0</v>
+      <c r="M79" t="s">
+        <v>644</v>
       </c>
       <c r="N79">
         <v>1</v>
@@ -8799,8 +8802,8 @@
       <c r="L80">
         <v>6</v>
       </c>
-      <c r="M80">
-        <v>0</v>
+      <c r="M80" t="s">
+        <v>644</v>
       </c>
       <c r="N80">
         <v>1</v>
@@ -8843,8 +8846,8 @@
       <c r="L81">
         <v>6</v>
       </c>
-      <c r="M81">
-        <v>0</v>
+      <c r="M81" t="s">
+        <v>644</v>
       </c>
       <c r="N81">
         <v>1</v>
@@ -8887,8 +8890,8 @@
       <c r="L82">
         <v>6</v>
       </c>
-      <c r="M82">
-        <v>0</v>
+      <c r="M82" t="s">
+        <v>644</v>
       </c>
       <c r="N82">
         <v>1</v>
@@ -8931,8 +8934,8 @@
       <c r="L83">
         <v>6</v>
       </c>
-      <c r="M83">
-        <v>0</v>
+      <c r="M83" t="s">
+        <v>644</v>
       </c>
       <c r="N83">
         <v>1</v>
@@ -8975,8 +8978,8 @@
       <c r="L84">
         <v>6</v>
       </c>
-      <c r="M84">
-        <v>0</v>
+      <c r="M84" t="s">
+        <v>644</v>
       </c>
       <c r="N84">
         <v>1</v>
@@ -9019,8 +9022,8 @@
       <c r="L85">
         <v>6</v>
       </c>
-      <c r="M85">
-        <v>0</v>
+      <c r="M85" t="s">
+        <v>644</v>
       </c>
       <c r="N85">
         <v>1</v>
@@ -9063,8 +9066,8 @@
       <c r="L86">
         <v>6</v>
       </c>
-      <c r="M86">
-        <v>0</v>
+      <c r="M86" t="s">
+        <v>644</v>
       </c>
       <c r="N86">
         <v>1</v>
@@ -9107,8 +9110,8 @@
       <c r="L87">
         <v>6</v>
       </c>
-      <c r="M87">
-        <v>0</v>
+      <c r="M87" t="s">
+        <v>644</v>
       </c>
       <c r="N87">
         <v>1</v>
@@ -9151,8 +9154,8 @@
       <c r="L88">
         <v>6</v>
       </c>
-      <c r="M88">
-        <v>0</v>
+      <c r="M88" t="s">
+        <v>644</v>
       </c>
       <c r="N88">
         <v>1</v>
@@ -9195,8 +9198,8 @@
       <c r="L89">
         <v>6</v>
       </c>
-      <c r="M89">
-        <v>0</v>
+      <c r="M89" t="s">
+        <v>644</v>
       </c>
       <c r="N89">
         <v>1</v>
@@ -9239,8 +9242,8 @@
       <c r="L90">
         <v>6</v>
       </c>
-      <c r="M90">
-        <v>0</v>
+      <c r="M90" t="s">
+        <v>644</v>
       </c>
       <c r="N90">
         <v>1</v>
@@ -9283,8 +9286,8 @@
       <c r="L91">
         <v>6</v>
       </c>
-      <c r="M91">
-        <v>0</v>
+      <c r="M91" t="s">
+        <v>644</v>
       </c>
       <c r="N91">
         <v>1</v>
@@ -9327,8 +9330,8 @@
       <c r="L92">
         <v>6</v>
       </c>
-      <c r="M92">
-        <v>0</v>
+      <c r="M92" t="s">
+        <v>644</v>
       </c>
       <c r="N92">
         <v>1</v>
@@ -9371,8 +9374,8 @@
       <c r="L93">
         <v>6</v>
       </c>
-      <c r="M93">
-        <v>0</v>
+      <c r="M93" t="s">
+        <v>644</v>
       </c>
       <c r="N93">
         <v>1</v>
@@ -9415,8 +9418,8 @@
       <c r="L94">
         <v>6</v>
       </c>
-      <c r="M94">
-        <v>0</v>
+      <c r="M94" t="s">
+        <v>644</v>
       </c>
       <c r="N94">
         <v>1</v>
@@ -9459,8 +9462,8 @@
       <c r="L95">
         <v>6</v>
       </c>
-      <c r="M95">
-        <v>0</v>
+      <c r="M95" t="s">
+        <v>644</v>
       </c>
       <c r="N95">
         <v>1</v>

</xml_diff>